<commit_message>
got all data for november
</commit_message>
<xml_diff>
--- a/excel_data/2020-11-04.xlsx
+++ b/excel_data/2020-11-04.xlsx
@@ -678,7 +678,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>1</c:v>
@@ -1989,7 +1989,7 @@
         <v>136</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3">

</xml_diff>